<commit_message>
Changed Secondary zip code to continue on error and fixed selectors . Login is now manual because of label printer issue. Moved file is now working.
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -139,58 +139,58 @@
     <x:t>SecondaryInsurance_ZipCode</x:t>
   </x:si>
   <x:si>
-    <x:t>2024-02-09</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5311</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17282310</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MM0000002108</x:t>
+    <x:t>2024-02-14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>271436</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13441336</x:t>
+  </x:si>
+  <x:si>
+    <x:t>921624</x:t>
   </x:si>
   <x:si>
     <x:t>Sagis DX (Ellkay)</x:t>
   </x:si>
   <x:si>
-    <x:t>Holzheimer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Elizabeth</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1956-06-10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Female</x:t>
-  </x:si>
-  <x:si>
-    <x:t>183 S SPIES RIDGE DR</x:t>
+    <x:t>BERNSTEIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MELVIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1947-06-08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Male</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1113 HAMPSTEAD LN</x:t>
   </x:si>
   <x:si>
     <x:t>TX</x:t>
   </x:si>
   <x:si>
-    <x:t>FREDERICKSBURG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>786242254</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9723438453</x:t>
+    <x:t>ALLEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>75013</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8327228681</x:t>
   </x:si>
   <x:si>
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>Julia Andrade,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Clear Creek Dermatology, Marble Falls</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Medicare of Texas</x:t>
+    <x:t>Christopher Stroud, MD,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(MK) Dallas Assoc Derm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MEDICARE PART B</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
SO RIGHT NOW I CHANGED THE REFERENCE TO in_strpatientsname which can allow the person to choose which file gets pulled . changed conditoins for stress address cont and for sub date.
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <x:si>
     <x:t>BillType</x:t>
   </x:si>
@@ -139,58 +139,61 @@
     <x:t>SecondaryInsurance_ZipCode</x:t>
   </x:si>
   <x:si>
-    <x:t>2024-02-14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>271436</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13441336</x:t>
-  </x:si>
-  <x:si>
-    <x:t>921624</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sagis DX (Ellkay)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BERNSTEIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MELVIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1947-06-08</x:t>
+    <x:t>2024-02-06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40402</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17500040</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16549</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sagis DX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TRESCH JR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ROBERT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>E</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1952-04-24</x:t>
   </x:si>
   <x:si>
     <x:t>Male</x:t>
   </x:si>
   <x:si>
-    <x:t>1113 HAMPSTEAD LN</x:t>
+    <x:t>7104 DOSWELL LN</x:t>
   </x:si>
   <x:si>
     <x:t>TX</x:t>
   </x:si>
   <x:si>
-    <x:t>ALLEN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>75013</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8327228681</x:t>
+    <x:t>AUSTIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>787392042</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5124238633</x:t>
   </x:si>
   <x:si>
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>Christopher Stroud, MD,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(MK) Dallas Assoc Derm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MEDICARE PART B</x:t>
+    <x:t>Leigha Sharp, MD,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SWDV- Austin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Medicare of Texas</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -667,38 +670,41 @@
       <x:c r="H2" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="L2" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="M2" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="N2" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="O2" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="P2" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="R2" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="S2" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="W2" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
CurrentRow location  message box  enabled. added an input dialgoue for the person to tell the bot which req to run . Input dialgoue is now the reference .
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <x:si>
     <x:t>BillType</x:t>
   </x:si>
@@ -145,76 +145,73 @@
     <x:t>2024-02-16</x:t>
   </x:si>
   <x:si>
-    <x:t>117781</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10302226</x:t>
-  </x:si>
-  <x:si>
-    <x:t>A ZIR001</x:t>
+    <x:t>33556</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32847311.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SHUBR000</x:t>
   </x:si>
   <x:si>
     <x:t>Sagis DX</x:t>
   </x:si>
   <x:si>
-    <x:t>ZIRKEL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ROBERT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1948-05-23</x:t>
+    <x:t>SHUMAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BRIAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>J</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1956-12-31</x:t>
   </x:si>
   <x:si>
     <x:t>Male</x:t>
   </x:si>
   <x:si>
-    <x:t>13622 EVERGREEN WAY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AUSTIN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>78737</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5128011998</x:t>
+    <x:t>PO BOX 1174</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ABITA SPRINGS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>704201174</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9856309533</x:t>
   </x:si>
   <x:si>
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>Daniel Carrasco, MD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sanova Dermatology Dripping Springs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ROBERT ZIRKEL</x:t>
+    <x:t>Stratton Beatrous Grisoli M.D.,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Baldone Reina Dermatology, APMC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BRIAN SHUMAN</x:t>
   </x:si>
   <x:si>
     <x:t>Self</x:t>
   </x:si>
   <x:si>
-    <x:t>Blue Cross Medicare Advantage Texas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ZZTULT5MM41H</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PO BOX 3686</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SCRANTON</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>185050686</x:t>
+    <x:t>Medicare of Louisiana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4NT5FH0HP64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Physicians Mutual Insurance Company</x:t>
+  </x:si>
+  <x:si>
+    <x:t>H730052094</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -694,59 +691,68 @@
       <x:c r="H2" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="N2" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="R2" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="S2" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="T2" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="U2" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="V2" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="M2" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="N2" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="O2" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="P2" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="Q2" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="R2" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="S2" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="T2" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="U2" s="0" t="s">
+      <x:c r="W2" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="Y2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AD2" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="W2" s="0" t="s">
+      <x:c r="AE2" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="Y2" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="Z2" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="AA2" s="0" t="s">
+      <x:c r="AF2" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AG2" s="0" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="AB2" s="0" t="s">
+      <x:c r="AI2" s="0" t="s">
         <x:v>63</x:v>
-      </x:c>
-      <x:c r="AC2" s="0" t="s">
-        <x:v>64</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
CurrentRow location enabled Bot may have read message box . added an input dialgoue for the person to tell which req to run . UPDATE BOT ON ORCH TOMORROW changed input dialogue to move file to see if that helps with naming conventions . instrpatient name for add queue for du queue.
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <x:si>
     <x:t>BillType</x:t>
   </x:si>
@@ -145,73 +145,70 @@
     <x:t>2024-02-16</x:t>
   </x:si>
   <x:si>
-    <x:t>33556</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32847311.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SHUBR000</x:t>
+    <x:t>20474</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21843299</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MM0000012163</x:t>
   </x:si>
   <x:si>
     <x:t>Sagis DX</x:t>
   </x:si>
   <x:si>
-    <x:t>SHUMAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BRIAN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>J</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1956-12-31</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Male</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PO BOX 1174</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ABITA SPRINGS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>704201174</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9856309533</x:t>
+    <x:t>Cardarelle Ross</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Joy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1950-06-08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Female</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5601 Spruce Ave</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Castle Rock</x:t>
+  </x:si>
+  <x:si>
+    <x:t>80104</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3038600948</x:t>
   </x:si>
   <x:si>
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>Stratton Beatrous Grisoli M.D.,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Baldone Reina Dermatology, APMC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BRIAN SHUMAN</x:t>
+    <x:t>Taylor Todd,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Clarity Dermatology - Castle Rock</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Joy Cardarelle Ross</x:t>
   </x:si>
   <x:si>
     <x:t>Self</x:t>
   </x:si>
   <x:si>
-    <x:t>Medicare of Louisiana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4NT5FH0HP64</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Physicians Mutual Insurance Company</x:t>
-  </x:si>
-  <x:si>
-    <x:t>H730052094</x:t>
+    <x:t>Medicare of Colorado</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9VD5TU8PW68</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AARP Medicare Supplement/Fixed Indemnity by UHC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01477099411</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -691,68 +688,59 @@
       <x:c r="H2" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="I2" s="0" t="s">
+      <x:c r="J2" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="s">
+      <x:c r="K2" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="K2" s="0" t="s">
+      <x:c r="L2" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="s">
+      <x:c r="M2" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="M2" s="0" t="s">
+      <x:c r="N2" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="N2" s="0" t="s">
+      <x:c r="O2" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="O2" s="0" t="s">
+      <x:c r="P2" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="P2" s="0" t="s">
+      <x:c r="Q2" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="Q2" s="0" t="s">
+      <x:c r="R2" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="R2" s="0" t="s">
+      <x:c r="S2" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="S2" s="0" t="s">
+      <x:c r="T2" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="T2" s="0" t="s">
+      <x:c r="U2" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="U2" s="0" t="s">
+      <x:c r="W2" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="V2" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="W2" s="0" t="s">
+      <x:c r="Y2" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="Y2" s="0" t="s">
+      <x:c r="AD2" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AE2" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="AG2" s="0" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="AD2" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="AE2" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="AF2" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="AG2" s="0" t="s">
+      <x:c r="AI2" s="0" t="s">
         <x:v>62</x:v>
-      </x:c>
-      <x:c r="AI2" s="0" t="s">
-        <x:v>63</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
instrpatient name for add queue for du queue. . updated selectors of site location. HAD TO FOLLOW ARGS THEY WERENT EVERYWHERE.
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -142,73 +142,73 @@
     <x:t>Third-Party Bill</x:t>
   </x:si>
   <x:si>
-    <x:t>2024-02-16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20474</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21843299</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MM0000012163</x:t>
+    <x:t>2024-02-14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33514</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29469205</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEWMA001</x:t>
   </x:si>
   <x:si>
     <x:t>Sagis DX</x:t>
   </x:si>
   <x:si>
-    <x:t>Cardarelle Ross</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Joy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1950-06-08</x:t>
+    <x:t>SEWARD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MARY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1954-10-20</x:t>
   </x:si>
   <x:si>
     <x:t>Female</x:t>
   </x:si>
   <x:si>
-    <x:t>5601 Spruce Ave</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Castle Rock</x:t>
-  </x:si>
-  <x:si>
-    <x:t>80104</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3038600948</x:t>
+    <x:t>826 AUTUMN PL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MANDEVILLE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>704716772</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5044603163</x:t>
   </x:si>
   <x:si>
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>Taylor Todd,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Clarity Dermatology - Castle Rock</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Joy Cardarelle Ross</x:t>
+    <x:t>Stratton Beatrous Grisoli M.D.,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Baldone Reina Dermatology, APMC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MARY SEWARD</x:t>
   </x:si>
   <x:si>
     <x:t>Self</x:t>
   </x:si>
   <x:si>
-    <x:t>Medicare of Colorado</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9VD5TU8PW68</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AARP Medicare Supplement/Fixed Indemnity by UHC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01477099411</x:t>
+    <x:t>Humana Health Plan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>X2284001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>H64587383</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -688,58 +688,55 @@
       <x:c r="H2" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="N2" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="R2" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="S2" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="T2" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="U2" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="V2" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="M2" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="N2" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="O2" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="P2" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="Q2" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="R2" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="S2" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="T2" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="U2" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
       <x:c r="W2" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="X2" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
       <x:c r="Y2" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="AD2" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="AE2" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="AG2" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="AI2" s="0" t="s">
         <x:v>62</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
had to do a switch for ezderm and default train more labels
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -20,87 +20,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
-  <x:si>
-    <x:t>BillType</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <x:si>
+    <x:t>RequisitionNumber</x:t>
   </x:si>
   <x:si>
     <x:t>CollectionDate</x:t>
   </x:si>
   <x:si>
-    <x:t>RequisitionNumber</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PMS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EMR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laboratory</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LastName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FirstName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MiddleName</x:t>
+    <x:t>OrderingPhysician</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hospital</x:t>
+  </x:si>
+  <x:si>
+    <x:t>City</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZipCode</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HomePhone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phys Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Patient Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gender</x:t>
   </x:si>
   <x:si>
     <x:t>DateOfBirth</x:t>
   </x:si>
   <x:si>
-    <x:t>Gender</x:t>
-  </x:si>
-  <x:si>
     <x:t>Address</x:t>
   </x:si>
   <x:si>
-    <x:t>State</x:t>
-  </x:si>
-  <x:si>
-    <x:t>City</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ZipCode</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HomePhone</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RequisitionDetails</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OrderingPhysician</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hospital</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PrimaryInsurance_SubscriberName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PrimaryInsurance_Relationship</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PrimaryInsurance_SubDOB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PrimaryInsurance_CompanyName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PrimaryInsurance_ContractNumber</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PrimaryInsurance_MemberID</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PrimaryInsurance_StreetAddress</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PrimaryInsurance_City</x:t>
+    <x:t>MRN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>External MRN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Primary Ins</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Primary Ins Num</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SecondaryInsurance_CompanyName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SecondaryInsurance_Num</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Num of Specimens</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Site Location 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Other 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Type Of Procedure 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Physical Exam 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Site Location 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Other 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Type Of Procedure 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Physical Exam 2</x:t>
   </x:si>
   <x:si>
     <x:t>PrimaryInsurance_State</x:t>
@@ -118,9 +118,6 @@
     <x:t>SecondaryInsurance_SubDOB</x:t>
   </x:si>
   <x:si>
-    <x:t>SecondaryInsurance_CompanyName</x:t>
-  </x:si>
-  <x:si>
     <x:t>SecondaryInsurance_ContractNumber</x:t>
   </x:si>
   <x:si>
@@ -139,76 +136,61 @@
     <x:t>SecondaryInsurance_ZipCode</x:t>
   </x:si>
   <x:si>
-    <x:t>Third-Party Bill</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2024-02-14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33514</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29469205</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SEWMA001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sagis DX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SEWARD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MARY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1954-10-20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Female</x:t>
-  </x:si>
-  <x:si>
-    <x:t>826 AUTUMN PL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MANDEVILLE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>704716772</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5044603163</x:t>
-  </x:si>
-  <x:si>
-    <x:t>table</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stratton Beatrous Grisoli M.D.,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Baldone Reina Dermatology, APMC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MARY SEWARD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Self</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Humana Health Plan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X2284001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>H64587383</x:t>
+    <x:t>REQUISITION:P2418L00AH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Erez A Minka</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vernon, TX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76384</x:t>
+  </x:si>
+  <x:si>
+    <x:t>940-687-3376</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4327 Barnett Road Wichita Falls, TX 763102303</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Boatman, Jason</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(M/41)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1982-09-09</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2231 14th St Vernon,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JABO0002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HMO Blue Shield Texas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>84980) (JEA014100810)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>= Medial</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Medial Neoplasm of uncertain behavior of skin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Biopsy (Tangential (Shave))</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pink papule (Forehead - Medial)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>405124601</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -642,102 +624,87 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="AG1" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="AH1" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="AH1" s="0" t="s">
+      <x:c r="AI1" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="AI1" s="0" t="s">
+      <x:c r="AJ1" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="AJ1" s="0" t="s">
+      <x:c r="AK1" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="AK1" s="0" t="s">
+      <x:c r="AL1" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="AL1" s="0" t="s">
+      <x:c r="AM1" s="0" t="s">
         <x:v>37</x:v>
-      </x:c>
-      <x:c r="AM1" s="0" t="s">
-        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:39">
       <x:c r="A2" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="J2" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
+      <x:c r="K2" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="I2" s="0" t="s">
+      <x:c r="L2" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="s">
+      <x:c r="M2" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="K2" s="0" t="s">
+      <x:c r="N2" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="s">
+      <x:c r="P2" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="M2" s="0" t="s">
+      <x:c r="T2" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="N2" s="0" t="s">
+      <x:c r="U2" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="O2" s="0" t="s">
+      <x:c r="V2" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="P2" s="0" t="s">
+      <x:c r="W2" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="Q2" s="0" t="s">
+      <x:c r="AB2" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="R2" s="0" t="s">
+      <x:c r="AC2" s="0" t="s">
         <x:v>56</x:v>
-      </x:c>
-      <x:c r="S2" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="T2" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="U2" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="V2" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="W2" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="X2" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="Y2" s="0" t="s">
-        <x:v>62</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
took out message box and Split((Split(InsurancePayer,":")(1).ToString),"(")(0).ToString in Enteraccession
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <x:si>
     <x:t>RequisitionNumber</x:t>
   </x:si>
@@ -136,16 +136,16 @@
     <x:t>SecondaryInsurance_ZipCode</x:t>
   </x:si>
   <x:si>
-    <x:t>REQUISITION:P2418L00AH</x:t>
+    <x:t>REQUISITION:P2318L01H0</x:t>
   </x:si>
   <x:si>
     <x:t>Erez A Minka</x:t>
   </x:si>
   <x:si>
-    <x:t>Vernon, TX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>76384</x:t>
+    <x:t>Wichita Falls,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76308</x:t>
   </x:si>
   <x:si>
     <x:t>940-687-3376</x:t>
@@ -154,37 +154,46 @@
     <x:t>4327 Barnett Road Wichita Falls, TX 763102303</x:t>
   </x:si>
   <x:si>
-    <x:t>Boatman, Jason</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(M/41)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1982-09-09</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2231 14th St Vernon,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JABO0002</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HMO Blue Shield Texas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>84980) (JEA014100810)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>= Medial</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Medial Neoplasm of uncertain behavior of skin</x:t>
+    <x:t>Askins, Sammie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(M/79)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1944-06-13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100 Chaparral Drive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SAAS0001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Medicare = Texas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(7WJ3UD1AE99)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Blue Shield = Texas Askins,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Anterior Left Upper Arm - Central</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Neoplasm of uncertain behavior of skin</x:t>
   </x:si>
   <x:si>
     <x:t>Biopsy (Tangential (Shave))</x:t>
   </x:si>
   <x:si>
-    <x:t>Pink papule (Forehead - Medial)</x:t>
+    <x:t>Pink papule (Anterior Left Upper Arm = Central)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Submandibular Neck - Left</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Exam: Pink papule (Submandibular Neck = Left)</x:t>
   </x:si>
   <x:si>
     <x:t>KY</x:t>
@@ -688,23 +697,38 @@
       <x:c r="P2" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
       <x:c r="T2" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="U2" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="V2" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="W2" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="X2" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="Y2" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="W2" s="0" t="s">
+      <x:c r="Z2" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
+      <x:c r="AA2" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
       <x:c r="AB2" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="AC2" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
changed input dialgoue location at end . Updated site location 2 other 2 etc for ezDerm because it was only doing one part of the 2nd page on vital.. Need to work on this.
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <x:si>
     <x:t>RequisitionNumber</x:t>
   </x:si>
@@ -136,49 +136,52 @@
     <x:t>SecondaryInsurance_ZipCode</x:t>
   </x:si>
   <x:si>
-    <x:t>REQUISITION:P2318L01H0</x:t>
+    <x:t>REQUISITION:P2418L001Y</x:t>
   </x:si>
   <x:si>
     <x:t>Erez A Minka</x:t>
   </x:si>
   <x:si>
-    <x:t>Wichita Falls,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>76308</x:t>
-  </x:si>
-  <x:si>
-    <x:t>940-687-3376</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4327 Barnett Road Wichita Falls, TX 763102303</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Askins, Sammie</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(M/79)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1944-06-13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100 Chaparral Drive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SAAS0001</x:t>
+    <x:t>lowa Park, TX 763678633</x:t>
+  </x:si>
+  <x:si>
+    <x:t>763678633</x:t>
+  </x:si>
+  <x:si>
+    <x:t>940-704-9644</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4327 Barnett Road Wichita Falls. TX 763102303</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Redclift, Reynold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L (M/78)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1945-05-23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11681 Longley Road</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RERE0001</x:t>
   </x:si>
   <x:si>
     <x:t>Medicare = Texas</x:t>
   </x:si>
   <x:si>
-    <x:t>(7WJ3UD1AE99)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Blue Shield = Texas Askins,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Anterior Left Upper Arm - Central</x:t>
+    <x:t>MR005) (2W51VF0GN34)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mutual of Omaha Insurance Company</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(72861188)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Right Suprascapular Back = Lateral</x:t>
   </x:si>
   <x:si>
     <x:t>Neoplasm of uncertain behavior of skin</x:t>
@@ -187,13 +190,16 @@
     <x:t>Biopsy (Tangential (Shave))</x:t>
   </x:si>
   <x:si>
-    <x:t>Pink papule (Anterior Left Upper Arm = Central)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Submandibular Neck - Left</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Exam: Pink papule (Submandibular Neck = Left)</x:t>
+    <x:t>Pink papule (Right Suprascapular Back - Lateral)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Right Ear = Descending Helix</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Helix Neoplasm of uncertain behavior of skin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Exam: Pink papule (Right Ear = Descending Helix)</x:t>
   </x:si>
   <x:si>
     <x:t>KY</x:t>
@@ -700,35 +706,38 @@
       <x:c r="Q2" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
+      <x:c r="R2" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
       <x:c r="T2" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="U2" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="V2" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="W2" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="X2" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="Y2" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Z2" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="X2" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="Y2" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="Z2" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
       <x:c r="AA2" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="AB2" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="AC2" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
For some reason the last update didnt work for the clicking but I changed it again .
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <x:si>
     <x:t>RequisitionNumber</x:t>
   </x:si>
@@ -136,76 +136,79 @@
     <x:t>SecondaryInsurance_ZipCode</x:t>
   </x:si>
   <x:si>
-    <x:t>REQUISITION:P2418L001Y</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Erez A Minka</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lowa Park, TX 763678633</x:t>
-  </x:si>
-  <x:si>
-    <x:t>763678633</x:t>
-  </x:si>
-  <x:si>
-    <x:t>940-704-9644</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4327 Barnett Road Wichita Falls. TX 763102303</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Redclift, Reynold</x:t>
-  </x:si>
-  <x:si>
-    <x:t>L (M/78)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1945-05-23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11681 Longley Road</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RERE0001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Medicare = Texas</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MR005) (2W51VF0GN34)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mutual of Omaha Insurance Company</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(72861188)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Right Suprascapular Back = Lateral</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Neoplasm of uncertain behavior of skin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Biopsy (Tangential (Shave))</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pink papule (Right Suprascapular Back - Lateral)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Right Ear = Descending Helix</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Helix Neoplasm of uncertain behavior of skin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Exam: Pink papule (Right Ear = Descending Helix)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>405124601</x:t>
+    <x:t>Third-Party Bill</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024-03-05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1039163</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16567886</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WED31500</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Christian</x:t>
+  </x:si>
+  <x:si>
+    <x:t>William</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1964-10-30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Male</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11386 68th St N</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>West Palm Beach</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33412</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5617236746</x:t>
+  </x:si>
+  <x:si>
+    <x:t>table</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jennifer Marshall, PA-C,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wellington WED</x:t>
+  </x:si>
+  <x:si>
+    <x:t>William Christian</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Self</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BCBS of FL Blueselar PPO/EPO/POS/FEP/PPC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>99999U6K</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VMAH45391700</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PO BOX 1798</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jacksonville</x:t>
+  </x:si>
+  <x:si>
+    <x:t>322310014</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -664,22 +667,22 @@
       <x:c r="A2" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
@@ -695,49 +698,49 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="N2" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="R2" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="S2" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="T2" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="U2" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="W2" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="X2" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="Y2" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="Z2" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="AA2" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AB2" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="O2" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="P2" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="Q2" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="R2" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="T2" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="U2" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="V2" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="W2" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="X2" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="Y2" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="Z2" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="AA2" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="AB2" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
       <x:c r="AC2" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
so i just redid the whole retry scopes for extraction . It started working for ezderm.Had to unlink to fix the site location parts .
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <x:si>
     <x:t>RequisitionNumber</x:t>
   </x:si>
@@ -136,79 +136,70 @@
     <x:t>SecondaryInsurance_ZipCode</x:t>
   </x:si>
   <x:si>
-    <x:t>Third-Party Bill</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2024-03-05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1039163</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16567886</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WED31500</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Christian</x:t>
-  </x:si>
-  <x:si>
-    <x:t>William</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1964-10-30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Male</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11386 68th St N</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>West Palm Beach</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33412</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5617236746</x:t>
-  </x:si>
-  <x:si>
-    <x:t>table</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jennifer Marshall, PA-C,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Wellington WED</x:t>
-  </x:si>
-  <x:si>
-    <x:t>William Christian</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Self</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BCBS of FL Blueselar PPO/EPO/POS/FEP/PPC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>99999U6K</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VMAH45391700</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PO BOX 1798</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jacksonville</x:t>
-  </x:si>
-  <x:si>
-    <x:t>322310014</x:t>
+    <x:t>REQUISITION:P2418L0007</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Erez A Minka</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76230</x:t>
+  </x:si>
+  <x:si>
+    <x:t>940-687-3376</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4327 Barnett Road Wichita Falls. TX 763102303</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hutson, Larry</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(M/67)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024-03-24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dx 150 Zipper Street Bowie, TX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LAHU0001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Medicare = Texas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(9A71WX2EA16)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>State Farm Hutson,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(HK4420994343)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Right Ear = Superior Helix 0.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Neoplasm of uncertain behavior of skin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Biopsy (Tangential (Shave))</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pink papule (Right Ear = Superior Helix)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Right Lateral Forearm =</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Central 0.720.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>303740800</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -667,80 +658,77 @@
       <x:c r="A2" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
+      <x:c r="J2" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="s">
+      <x:c r="K2" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="K2" s="0" t="s">
+      <x:c r="L2" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="s">
+      <x:c r="M2" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="M2" s="0" t="s">
+      <x:c r="N2" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="N2" s="0" t="s">
+      <x:c r="P2" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="O2" s="0" t="s">
+      <x:c r="Q2" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="P2" s="0" t="s">
+      <x:c r="R2" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="Q2" s="0" t="s">
+      <x:c r="T2" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="R2" s="0" t="s">
+      <x:c r="U2" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="S2" s="0" t="s">
+      <x:c r="V2" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="T2" s="0" t="s">
+      <x:c r="W2" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="U2" s="0" t="s">
+      <x:c r="X2" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="W2" s="0" t="s">
+      <x:c r="Y2" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="Z2" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="AA2" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="X2" s="0" t="s">
+      <x:c r="AB2" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="Y2" s="0" t="s">
+      <x:c r="AC2" s="0" t="s">
         <x:v>59</x:v>
-      </x:c>
-      <x:c r="Z2" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="AA2" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="AB2" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="AC2" s="0" t="s">
-        <x:v>62</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
-Added secondary insurance and added those 2 items into the AddtoQueue DOESN'T CATCH SECONDARY INSURANCE IF PATIENT HAS ONE  - Added req number back STILL MESSES UP THE ADDRESS     -.replace for secondary policy # and payor () and =
</commit_message>
<xml_diff>
--- a/TESToutExtractResults.xlsx
+++ b/TESToutExtractResults.xlsx
@@ -196,10 +196,10 @@
     <x:t>Central 0.720.6</x:t>
   </x:si>
   <x:si>
-    <x:t>GA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>303740800</x:t>
+    <x:t>CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>802175747</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>